<commit_message>
modification PAN + modif Ultiboard + update pieces
correction des erreurs du Ultiboard. Mise à jour des pieces en stock.
Création d'un PAN
</commit_message>
<xml_diff>
--- a/Tableau_pieces_en_stock.xlsx
+++ b/Tableau_pieces_en_stock.xlsx
@@ -17,11 +17,12 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="137">
   <si>
     <t>INVENTAIRE DES PIÈCES DISPONIBLES</t>
   </si>
@@ -243,6 +244,195 @@
   </si>
   <si>
     <t>Jumper</t>
+  </si>
+  <si>
+    <t>Nouvelle commande</t>
+  </si>
+  <si>
+    <t>PIC 18f46J50</t>
+  </si>
+  <si>
+    <t>microchip</t>
+  </si>
+  <si>
+    <t>PIC18F45J50-I/PT</t>
+  </si>
+  <si>
+    <t>Switch slide</t>
+  </si>
+  <si>
+    <t>JS202011SCQN</t>
+  </si>
+  <si>
+    <t>micro USB-B</t>
+  </si>
+  <si>
+    <t>10118192-0001LF</t>
+  </si>
+  <si>
+    <t>FCI</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>CC0805ZKY5V6BB106</t>
+  </si>
+  <si>
+    <t>Abracon LLC</t>
+  </si>
+  <si>
+    <t>AB26TRQ-32.768KHZ-T</t>
+  </si>
+  <si>
+    <t>Écran</t>
+  </si>
+  <si>
+    <t>RC0805JR-0736KL</t>
+  </si>
+  <si>
+    <t>Chargeur</t>
+  </si>
+  <si>
+    <t>MCP73871-2CCI/ML</t>
+  </si>
+  <si>
+    <t>Régulateur</t>
+  </si>
+  <si>
+    <t>LM3671MF-3.3/NOPB</t>
+  </si>
+  <si>
+    <t>PTS645SM43SMTR92 LFS</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>3,3V</t>
+  </si>
+  <si>
+    <t>CL21F104ZBCNNNC</t>
+  </si>
+  <si>
+    <t>RC0805JR-07110KL</t>
+  </si>
+  <si>
+    <t>110k 5%</t>
+  </si>
+  <si>
+    <t>Stackpole</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD40k2</t>
+  </si>
+  <si>
+    <t>40,2k 1%</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD10k0</t>
+  </si>
+  <si>
+    <t>10k 1%</t>
+  </si>
+  <si>
+    <t>Bobine</t>
+  </si>
+  <si>
+    <t>TDK corporation</t>
+  </si>
+  <si>
+    <t>MLZ2012A2R2M</t>
+  </si>
+  <si>
+    <t>2,2uH 650mA 150ohm</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD2k00</t>
+  </si>
+  <si>
+    <t>2k 1%</t>
+  </si>
+  <si>
+    <t>CC0805ZRY5V6BB475</t>
+  </si>
+  <si>
+    <t>4,7uF</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD1k00</t>
+  </si>
+  <si>
+    <t>1k 1%</t>
+  </si>
+  <si>
+    <t>APT2012EC</t>
+  </si>
+  <si>
+    <t>rouge</t>
+  </si>
+  <si>
+    <t>APT2012SGC</t>
+  </si>
+  <si>
+    <t>vert</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>L0603C3N9SRMST</t>
+  </si>
+  <si>
+    <t>JONATHAN</t>
+  </si>
+  <si>
+    <t>AVX</t>
+  </si>
+  <si>
+    <t>HLC025R6BTTR</t>
+  </si>
+  <si>
+    <t>EPCOS</t>
+  </si>
+  <si>
+    <t>B82496C3829J</t>
+  </si>
+  <si>
+    <t>2 for JONATHAN</t>
+  </si>
+  <si>
+    <t>(1 brulé)</t>
+  </si>
+  <si>
+    <t>Colonne1</t>
+  </si>
+  <si>
+    <t>Colonne2</t>
+  </si>
+  <si>
+    <t>Colonne3</t>
+  </si>
+  <si>
+    <t>Colonne4</t>
+  </si>
+  <si>
+    <t>Colonne5</t>
+  </si>
+  <si>
+    <t>Colonne6</t>
+  </si>
+  <si>
+    <t>Colonne7</t>
+  </si>
+  <si>
+    <t>Colonne8</t>
+  </si>
+  <si>
+    <t>36k 5%</t>
+  </si>
+  <si>
+    <t>(2 jettés)</t>
   </si>
 </sst>
 </file>
@@ -283,7 +473,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -313,8 +503,47 @@
       <right style="thin">
         <color auto="1"/>
       </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -324,6 +553,39 @@
       <right style="thin">
         <color auto="1"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -334,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -350,21 +612,212 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -375,6 +828,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A34:H57" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="A34:H57"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Colonne1" dataDxfId="7"/>
+    <tableColumn id="2" name="Colonne2" dataDxfId="6"/>
+    <tableColumn id="3" name="Colonne3" dataDxfId="5"/>
+    <tableColumn id="4" name="Colonne4" dataDxfId="4"/>
+    <tableColumn id="5" name="Colonne5" dataDxfId="3"/>
+    <tableColumn id="6" name="Colonne6" dataDxfId="2"/>
+    <tableColumn id="7" name="Colonne7" dataDxfId="1"/>
+    <tableColumn id="8" name="Colonne8" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -640,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,39 +1157,40 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="25.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
       <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="13" t="s">
         <v>71</v>
       </c>
       <c r="I5" s="4"/>
@@ -772,7 +1243,10 @@
         <v>9.02</v>
       </c>
       <c r="H7" s="3">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -824,7 +1298,7 @@
         <v>2.04</v>
       </c>
       <c r="H9" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -899,7 +1373,7 @@
         <v>9.84</v>
       </c>
       <c r="H12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -924,7 +1398,7 @@
         <v>6.9599999999999991</v>
       </c>
       <c r="H13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -949,7 +1423,7 @@
         <v>4.0500000000000007</v>
       </c>
       <c r="H14" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -975,8 +1449,8 @@
         <f t="shared" si="0"/>
         <v>7.0000000000000009</v>
       </c>
-      <c r="H15" s="12">
-        <v>2</v>
+      <c r="H15" s="10">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1002,11 +1476,11 @@
         <f t="shared" si="0"/>
         <v>7.0000000000000009</v>
       </c>
-      <c r="H16" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>38</v>
       </c>
@@ -1029,11 +1503,11 @@
         <f t="shared" si="0"/>
         <v>24.8</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -1056,11 +1530,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H18" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
@@ -1083,11 +1557,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H19" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
@@ -1110,11 +1584,14 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H20" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="10">
+        <v>18</v>
+      </c>
+      <c r="I20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>50</v>
       </c>
@@ -1137,11 +1614,11 @@
         <f t="shared" si="0"/>
         <v>2.85</v>
       </c>
-      <c r="H21" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>50</v>
       </c>
@@ -1164,11 +1641,11 @@
         <f t="shared" si="0"/>
         <v>2.85</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>50</v>
       </c>
@@ -1191,11 +1668,11 @@
         <f t="shared" si="0"/>
         <v>2.85</v>
       </c>
-      <c r="H23" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>58</v>
       </c>
@@ -1216,11 +1693,11 @@
         <f t="shared" si="0"/>
         <v>13.26</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>61</v>
       </c>
@@ -1243,11 +1720,11 @@
         <f t="shared" si="0"/>
         <v>4.9400000000000004</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>65</v>
       </c>
@@ -1263,15 +1740,15 @@
       <c r="G26" s="5">
         <v>0</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="12" t="s">
         <v>67</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -1290,11 +1767,11 @@
         <f>E27*F27</f>
         <v>6.75</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>70</v>
       </c>
@@ -1303,12 +1780,12 @@
         <v>175.32999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>73</v>
       </c>
@@ -1322,6 +1799,528 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3">
+        <v>12</v>
+      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3">
+        <v>20</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3">
+        <v>13</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3">
+        <v>25</v>
+      </c>
+      <c r="G38" s="3"/>
+      <c r="H38" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3">
+        <v>15</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3">
+        <v>6</v>
+      </c>
+      <c r="G40" s="3"/>
+      <c r="H40" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3">
+        <v>10</v>
+      </c>
+      <c r="G41" s="3"/>
+      <c r="H41" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3">
+        <v>8</v>
+      </c>
+      <c r="G42" s="3"/>
+      <c r="H42" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3">
+        <v>10</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3">
+        <v>15</v>
+      </c>
+      <c r="G44" s="3"/>
+      <c r="H44" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3">
+        <v>50</v>
+      </c>
+      <c r="G45" s="3"/>
+      <c r="H45" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3">
+        <v>10</v>
+      </c>
+      <c r="G46" s="3"/>
+      <c r="H46" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3">
+        <v>10</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3">
+        <v>10</v>
+      </c>
+      <c r="G48" s="3"/>
+      <c r="H48" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3">
+        <v>10</v>
+      </c>
+      <c r="G49" s="3"/>
+      <c r="H49" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3">
+        <v>10</v>
+      </c>
+      <c r="G50" s="3"/>
+      <c r="H50" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3">
+        <v>25</v>
+      </c>
+      <c r="G51" s="3"/>
+      <c r="H51" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3">
+        <v>100</v>
+      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="16">
+        <v>2</v>
+      </c>
+      <c r="I52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3">
+        <v>10</v>
+      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="16"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3">
+        <v>10</v>
+      </c>
+      <c r="G54" s="3"/>
+      <c r="H54" s="16"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3">
+        <v>2</v>
+      </c>
+      <c r="G55" s="3"/>
+      <c r="H55" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3">
+        <v>2</v>
+      </c>
+      <c r="G56" s="3"/>
+      <c r="H56" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21">
+        <v>2</v>
+      </c>
+      <c r="G57" s="21"/>
+      <c r="H57" s="22">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1330,6 +2329,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
schéma du PCB étudiant
Le schéma multisim et ultiboard de la carte étudiante est terminée
(fonctionnelle, mais non optimisé)
</commit_message>
<xml_diff>
--- a/Tableau_pieces_en_stock.xlsx
+++ b/Tableau_pieces_en_stock.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\GitHub\243-510-A15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu\Documents\GitHub\243-510-A15\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8148"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -438,7 +437,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -619,9 +618,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -630,6 +626,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,6 +783,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -791,15 +799,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -831,7 +830,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A34:H57" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A34:H57" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A34:H57"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Colonne1" dataDxfId="7"/>
@@ -1112,24 +1111,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875"/>
-    <col min="2" max="2" width="21.5703125"/>
+    <col min="1" max="1" width="19.88671875"/>
+    <col min="2" max="2" width="21.5546875"/>
     <col min="3" max="4" width="33"/>
-    <col min="5" max="5" width="10.5703125"/>
-    <col min="6" max="6" width="10.42578125"/>
-    <col min="7" max="7" width="15.85546875"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875"/>
-    <col min="10" max="1025" width="10.5703125"/>
+    <col min="5" max="5" width="10.5546875"/>
+    <col min="6" max="6" width="10.44140625"/>
+    <col min="7" max="7" width="15.88671875"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875"/>
+    <col min="10" max="1025" width="10.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1138,7 +1137,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1147,7 +1146,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1156,19 +1155,19 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="25.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -1196,7 +1195,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1221,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1249,7 +1248,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -1274,7 +1273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
@@ -1326,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
@@ -1351,7 +1350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
@@ -1376,7 +1375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
@@ -1401,7 +1400,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>30</v>
       </c>
@@ -1426,7 +1425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>33</v>
       </c>
@@ -1453,7 +1452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>33</v>
       </c>
@@ -1480,7 +1479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>38</v>
       </c>
@@ -1507,7 +1506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -1534,7 +1533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
@@ -1561,7 +1560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
@@ -1591,7 +1590,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>50</v>
       </c>
@@ -1618,7 +1617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>50</v>
       </c>
@@ -1645,7 +1644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>50</v>
       </c>
@@ -1672,7 +1671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>58</v>
       </c>
@@ -1697,7 +1696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>61</v>
       </c>
@@ -1724,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>65</v>
       </c>
@@ -1744,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>66</v>
       </c>
@@ -1771,7 +1770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F29" t="s">
         <v>70</v>
       </c>
@@ -1780,12 +1779,12 @@
         <v>175.32999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>73</v>
       </c>
@@ -1801,39 +1800,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="G34" s="18" t="s">
+      <c r="G34" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="H34" s="19" t="s">
+      <c r="H34" s="18" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
         <v>75</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -1848,12 +1847,12 @@
         <v>12</v>
       </c>
       <c r="G35" s="3"/>
-      <c r="H35" s="16">
+      <c r="H35" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="14" t="s">
         <v>78</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -1868,12 +1867,12 @@
         <v>20</v>
       </c>
       <c r="G36" s="3"/>
-      <c r="H36" s="16">
+      <c r="H36" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="14" t="s">
         <v>80</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1888,12 +1887,12 @@
         <v>13</v>
       </c>
       <c r="G37" s="3"/>
-      <c r="H37" s="16">
+      <c r="H37" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -1910,12 +1909,12 @@
         <v>25</v>
       </c>
       <c r="G38" s="3"/>
-      <c r="H38" s="16">
+      <c r="H38" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -1930,12 +1929,12 @@
         <v>15</v>
       </c>
       <c r="G39" s="3"/>
-      <c r="H39" s="16">
+      <c r="H39" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="14" t="s">
         <v>87</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -1950,12 +1949,12 @@
         <v>6</v>
       </c>
       <c r="G40" s="3"/>
-      <c r="H40" s="16">
+      <c r="H40" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -1972,12 +1971,12 @@
         <v>10</v>
       </c>
       <c r="G41" s="3"/>
-      <c r="H41" s="16">
+      <c r="H41" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="14" t="s">
         <v>89</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -1992,12 +1991,12 @@
         <v>8</v>
       </c>
       <c r="G42" s="3"/>
-      <c r="H42" s="16">
+      <c r="H42" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
         <v>91</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2014,12 +2013,12 @@
         <v>10</v>
       </c>
       <c r="G43" s="3"/>
-      <c r="H43" s="16">
+      <c r="H43" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -2034,12 +2033,12 @@
         <v>15</v>
       </c>
       <c r="G44" s="3"/>
-      <c r="H44" s="16">
+      <c r="H44" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -2056,12 +2055,12 @@
         <v>50</v>
       </c>
       <c r="G45" s="3"/>
-      <c r="H45" s="16">
+      <c r="H45" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -2078,12 +2077,12 @@
         <v>10</v>
       </c>
       <c r="G46" s="3"/>
-      <c r="H46" s="16">
+      <c r="H46" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -2100,12 +2099,12 @@
         <v>10</v>
       </c>
       <c r="G47" s="3"/>
-      <c r="H47" s="16">
+      <c r="H47" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -2122,12 +2121,12 @@
         <v>10</v>
       </c>
       <c r="G48" s="3"/>
-      <c r="H48" s="16">
+      <c r="H48" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="14" t="s">
         <v>104</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -2144,12 +2143,12 @@
         <v>10</v>
       </c>
       <c r="G49" s="3"/>
-      <c r="H49" s="16">
+      <c r="H49" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -2166,12 +2165,12 @@
         <v>10</v>
       </c>
       <c r="G50" s="3"/>
-      <c r="H50" s="16">
+      <c r="H50" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -2188,12 +2187,12 @@
         <v>25</v>
       </c>
       <c r="G51" s="3"/>
-      <c r="H51" s="16">
+      <c r="H51" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B52" s="3" t="s">
@@ -2210,15 +2209,15 @@
         <v>100</v>
       </c>
       <c r="G52" s="3"/>
-      <c r="H52" s="16">
+      <c r="H52" s="15">
         <v>2</v>
       </c>
       <c r="I52" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="14" t="s">
         <v>50</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -2235,10 +2234,10 @@
         <v>10</v>
       </c>
       <c r="G53" s="3"/>
-      <c r="H53" s="16"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+      <c r="H53" s="15"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="14" t="s">
         <v>50</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -2255,10 +2254,10 @@
         <v>10</v>
       </c>
       <c r="G54" s="3"/>
-      <c r="H54" s="16"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
+      <c r="H54" s="15"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="14" t="s">
         <v>104</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -2275,12 +2274,12 @@
         <v>2</v>
       </c>
       <c r="G55" s="3"/>
-      <c r="H55" s="16">
+      <c r="H55" s="15">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="14" t="s">
         <v>104</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -2297,29 +2296,29 @@
         <v>2</v>
       </c>
       <c r="G56" s="3"/>
-      <c r="H56" s="16">
+      <c r="H56" s="15">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="20" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="D57" s="21" t="s">
+      <c r="D57" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21">
+      <c r="E57" s="20"/>
+      <c r="F57" s="20">
         <v>2</v>
       </c>
-      <c r="G57" s="21"/>
-      <c r="H57" s="22">
+      <c r="G57" s="20"/>
+      <c r="H57" s="21">
         <v>2</v>
       </c>
     </row>
@@ -2341,9 +2340,9 @@
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="10.5703125"/>
+    <col min="1" max="1025" width="10.5546875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2357,9 +2356,9 @@
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="10.5703125"/>
+    <col min="1" max="1025" width="10.5546875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>